<commit_message>
Adjusted the axis titles and data to match. It had revenue data with age data and that isn't correct
</commit_message>
<xml_diff>
--- a/SignalRChat/wwwroot/Uploads/SalesData.xlsx
+++ b/SignalRChat/wwwroot/Uploads/SalesData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive - James Madison University (Dukes)\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE83EABF-5404-4609-AA41-08CBC63D343F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC85045-CF53-4E2B-ADDB-78029225C5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7545" yWindow="2655" windowWidth="7500" windowHeight="11475" xr2:uid="{3FE44B22-F5B9-4CDB-8748-18897BF6B403}"/>
+    <workbookView xWindow="180" yWindow="3195" windowWidth="15675" windowHeight="11475" xr2:uid="{3FE44B22-F5B9-4CDB-8748-18897BF6B403}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +431,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>50000</v>
       </c>
       <c r="B2">
         <v>22</v>
@@ -439,7 +439,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>13456</v>
       </c>
       <c r="B3">
         <v>55</v>
@@ -447,7 +447,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>134567</v>
       </c>
       <c r="B4">
         <v>43</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>76544</v>
       </c>
       <c r="B5">
         <v>77</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>357373</v>
       </c>
       <c r="B6">
         <v>86</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>263573</v>
       </c>
       <c r="B7">
         <v>31</v>

</xml_diff>